<commit_message>
Training code compatibility optimization for Emperor data
</commit_message>
<xml_diff>
--- a/sessions_summary.xlsx
+++ b/sessions_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Storage\MATLAB\ThalamocorticalLoop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658E2ECE-326A-45EC-A2E5-F0A27A67AD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9482289B-BD0D-427B-9EB8-2F455AFCBB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{56367E76-6CBF-4746-8F91-48887379FCA8}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="14490" firstSheet="1" activeTab="3" xr2:uid="{56367E76-6CBF-4746-8F91-48887379FCA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="146">
   <si>
     <t>P3</t>
   </si>
@@ -432,13 +432,49 @@
   </si>
   <si>
     <t>8: thal only</t>
+  </si>
+  <si>
+    <t>Thalamus data lost in PreRestOpen (not affecting cortex)</t>
+  </si>
+  <si>
+    <t>01092026-008</t>
+  </si>
+  <si>
+    <t>01092026-001</t>
+  </si>
+  <si>
+    <t>01162026-008</t>
+  </si>
+  <si>
+    <t>01162026-001</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>L0</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>L7</t>
+  </si>
+  <si>
+    <t>L6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,6 +499,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1011,7 +1053,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1171,36 +1213,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1256,6 +1268,63 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1574,7 +1643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E51CD7-F882-46FB-A302-DE4F0A9E1B83}">
   <dimension ref="B3:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
@@ -1582,40 +1651,40 @@
   <cols>
     <col min="2" max="2" width="16.54296875" customWidth="1"/>
     <col min="3" max="3" width="13.1796875" customWidth="1"/>
-    <col min="4" max="6" width="12.81640625" style="115" customWidth="1"/>
+    <col min="4" max="6" width="12.81640625" style="105" customWidth="1"/>
     <col min="7" max="11" width="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="93" t="s">
+      <c r="C4" s="114" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="90" t="s">
+      <c r="D4" s="111" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="95" t="s">
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="113"/>
+      <c r="H4" s="116" t="s">
         <v>90</v>
       </c>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="92"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="113"/>
     </row>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="94"/>
-      <c r="D5" s="116" t="s">
+      <c r="C5" s="115"/>
+      <c r="D5" s="106" t="s">
         <v>129</v>
       </c>
-      <c r="E5" s="117" t="s">
+      <c r="E5" s="107" t="s">
         <v>130</v>
       </c>
-      <c r="F5" s="118" t="s">
+      <c r="F5" s="108" t="s">
         <v>131</v>
       </c>
-      <c r="G5" s="119" t="s">
+      <c r="G5" s="109" t="s">
         <v>104</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -1635,16 +1704,16 @@
       <c r="C6" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="102">
+      <c r="D6" s="92">
         <v>5</v>
       </c>
-      <c r="E6" s="113">
+      <c r="E6" s="103">
         <v>8</v>
       </c>
-      <c r="F6" s="104">
+      <c r="F6" s="94">
         <v>5</v>
       </c>
-      <c r="G6" s="105">
+      <c r="G6" s="95">
         <v>18</v>
       </c>
       <c r="H6" s="58"/>
@@ -1656,16 +1725,16 @@
       <c r="C7" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="114" t="s">
+      <c r="D7" s="104" t="s">
         <v>133</v>
       </c>
-      <c r="E7" s="106">
+      <c r="E7" s="96">
         <v>1</v>
       </c>
-      <c r="F7" s="107">
+      <c r="F7" s="97">
         <v>1</v>
       </c>
-      <c r="G7" s="108">
+      <c r="G7" s="98">
         <v>10</v>
       </c>
       <c r="H7" s="53"/>
@@ -1677,16 +1746,16 @@
       <c r="C8" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="109">
+      <c r="D8" s="99">
         <v>0</v>
       </c>
-      <c r="E8" s="110">
+      <c r="E8" s="100">
         <v>0</v>
       </c>
-      <c r="F8" s="111" t="s">
+      <c r="F8" s="101" t="s">
         <v>132</v>
       </c>
-      <c r="G8" s="112">
+      <c r="G8" s="102">
         <v>3</v>
       </c>
       <c r="H8" s="56"/>
@@ -1696,9 +1765,9 @@
     </row>
     <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="72"/>
-      <c r="D9" s="116"/>
-      <c r="E9" s="117"/>
-      <c r="F9" s="118"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="108"/>
       <c r="G9" s="72"/>
       <c r="H9" s="3"/>
       <c r="I9" s="73"/>
@@ -1706,15 +1775,15 @@
       <c r="K9" s="72"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="110" t="s">
         <v>88</v>
       </c>
       <c r="C10" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="102"/>
-      <c r="E10" s="103"/>
-      <c r="F10" s="104"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="94"/>
       <c r="G10" s="57"/>
       <c r="H10" s="58"/>
       <c r="I10" s="74"/>
@@ -1722,13 +1791,13 @@
       <c r="K10" s="57"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="89"/>
+      <c r="B11" s="110"/>
       <c r="C11" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="109"/>
-      <c r="E11" s="110"/>
-      <c r="F11" s="111"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="101"/>
       <c r="G11" s="55"/>
       <c r="H11" s="56"/>
       <c r="I11" s="71"/>
@@ -1736,23 +1805,23 @@
       <c r="K11" s="55"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="D14" s="89" t="s">
+      <c r="D14" s="110" t="s">
         <v>122</v>
       </c>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="89" t="s">
+      <c r="E14" s="110"/>
+      <c r="F14" s="110"/>
+      <c r="G14" s="110" t="s">
         <v>123</v>
       </c>
-      <c r="H14" s="89"/>
-      <c r="I14" s="89"/>
-      <c r="J14" s="89" t="s">
+      <c r="H14" s="110"/>
+      <c r="I14" s="110"/>
+      <c r="J14" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="89" t="s">
+      <c r="K14" s="110" t="s">
         <v>11</v>
       </c>
-      <c r="L14" s="89" t="s">
+      <c r="L14" s="110" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1775,9 +1844,9 @@
       <c r="I15" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="89"/>
+      <c r="J15" s="110"/>
+      <c r="K15" s="110"/>
+      <c r="L15" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1799,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50FFE666-9548-4978-AD59-82159C4DB165}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8:O9"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1814,7 +1883,7 @@
     <col min="11" max="11" width="5.453125" style="1"/>
     <col min="12" max="12" width="4.1796875" style="1" customWidth="1"/>
     <col min="13" max="13" width="5.26953125" customWidth="1"/>
-    <col min="14" max="14" width="42.26953125" customWidth="1"/>
+    <col min="14" max="14" width="55.26953125" customWidth="1"/>
     <col min="15" max="15" width="31" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1831,21 +1900,21 @@
       <c r="D1" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="96" t="s">
+      <c r="E1" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="96"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="98" t="s">
+      <c r="F1" s="117"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="96"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="98" t="s">
+      <c r="I1" s="117"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="119" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="96"/>
-      <c r="M1" s="97"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="118"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="44" t="s">
@@ -2398,6 +2467,9 @@
       </c>
       <c r="M14" s="3">
         <v>54</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="O14" t="s">
         <v>118</v>
@@ -2978,23 +3050,23 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="99"/>
-      <c r="B8" s="100" t="s">
+      <c r="A8" s="89"/>
+      <c r="B8" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="100" t="s">
+      <c r="C8" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="101" t="s">
+      <c r="D8" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="100"/>
-      <c r="F8" s="100"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="100" t="s">
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="90" t="s">
         <v>120</v>
       </c>
-      <c r="I8" s="100" t="s">
+      <c r="I8" s="90" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3072,10 +3144,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD31B0A-8ACD-468E-8C67-02F9624BD3CF}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3084,11 +3156,11 @@
     <col min="2" max="2" width="16.90625" style="50" customWidth="1"/>
     <col min="3" max="3" width="14.453125" style="50" customWidth="1"/>
     <col min="4" max="4" width="23.1796875" style="50" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" style="50" customWidth="1"/>
-    <col min="6" max="16384" width="29.81640625" style="50"/>
+    <col min="5" max="13" width="6.453125" style="50" customWidth="1"/>
+    <col min="14" max="16384" width="29.81640625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="59" t="s">
         <v>114</v>
       </c>
@@ -3098,14 +3170,26 @@
       <c r="C1" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="62"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E1" s="132" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="132"/>
+      <c r="J1" s="132"/>
+      <c r="K1" s="132" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="132"/>
+      <c r="M1" s="132"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="63" t="s">
         <v>108</v>
       </c>
@@ -3118,9 +3202,35 @@
       <c r="D2" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="64"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E2" s="120" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="120" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="121">
+        <v>8</v>
+      </c>
+      <c r="H2" s="122" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" s="123" t="s">
+        <v>143</v>
+      </c>
+      <c r="J2" s="124">
+        <v>3</v>
+      </c>
+      <c r="K2" s="125" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="120" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>109</v>
       </c>
@@ -3133,9 +3243,35 @@
       <c r="D3" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="64"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E3" s="120" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="120" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="121">
+        <v>12</v>
+      </c>
+      <c r="H3" s="122" t="s">
+        <v>142</v>
+      </c>
+      <c r="I3" s="123" t="s">
+        <v>143</v>
+      </c>
+      <c r="J3" s="124">
+        <v>10</v>
+      </c>
+      <c r="K3" s="125" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="120" t="s">
+        <v>144</v>
+      </c>
+      <c r="M3" s="124">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="63" t="s">
         <v>110</v>
       </c>
@@ -3148,39 +3284,137 @@
       <c r="D4" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="64"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="63"/>
-      <c r="D5" s="64"/>
-      <c r="G5" s="64"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="63"/>
-      <c r="D6" s="64"/>
-      <c r="G6" s="64"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E4" s="120" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4" s="120" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="121">
+        <v>20</v>
+      </c>
+      <c r="H4" s="122" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="123" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="124">
+        <v>9</v>
+      </c>
+      <c r="K4" s="125" t="s">
+        <v>142</v>
+      </c>
+      <c r="L4" s="120" t="s">
+        <v>145</v>
+      </c>
+      <c r="M4" s="124">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="64" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="120" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" s="120" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="121">
+        <v>9</v>
+      </c>
+      <c r="H5" s="122" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="123" t="s">
+        <v>143</v>
+      </c>
+      <c r="J5" s="124">
+        <v>11</v>
+      </c>
+      <c r="K5" s="125" t="s">
+        <v>142</v>
+      </c>
+      <c r="L5" s="120" t="s">
+        <v>145</v>
+      </c>
+      <c r="M5" s="124">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="126" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="126" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="127">
+        <v>18</v>
+      </c>
+      <c r="H6" s="128" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" s="129" t="s">
+        <v>143</v>
+      </c>
+      <c r="J6" s="130">
+        <v>17</v>
+      </c>
+      <c r="K6" s="131" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="126" t="s">
+        <v>145</v>
+      </c>
+      <c r="M6" s="130">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="63"/>
       <c r="D7" s="64"/>
       <c r="G7" s="64"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="63"/>
       <c r="D8" s="64"/>
       <c r="G8" s="64"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="63"/>
       <c r="D9" s="64"/>
       <c r="G9" s="64"/>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="63"/>
       <c r="D10" s="64"/>
       <c r="G10" s="64"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="68"/>
       <c r="B11" s="61"/>
       <c r="C11" s="61"/>
@@ -3189,7 +3423,7 @@
       <c r="F11" s="61"/>
       <c r="G11" s="62"/>
     </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="65"/>
       <c r="B12" s="66"/>
       <c r="C12" s="66"/>
@@ -3199,6 +3433,11 @@
       <c r="G12" s="67"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
new data: 01232026, 01302026
</commit_message>
<xml_diff>
--- a/sessions_summary.xlsx
+++ b/sessions_summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Storage\MATLAB\ThalamocorticalLoop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pri\Storage\Projects\ThalamoCorticalNetwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A12FE6B-FB1B-4050-90A7-A74066D4EC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF86137-160F-4FE0-9358-900430DDCBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" firstSheet="1" activeTab="3" xr2:uid="{56367E76-6CBF-4746-8F91-48887379FCA8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{56367E76-6CBF-4746-8F91-48887379FCA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -20,17 +20,28 @@
     <sheet name="Lemmy-Kaining" sheetId="3" r:id="rId5"/>
     <sheet name="Slayer-Kaining" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="150">
   <si>
     <t>P3</t>
   </si>
@@ -477,6 +488,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Excluded: Post no eye-close</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1279,6 +1293,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1309,40 +1347,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6D6D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1355,9 +1376,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1395,7 +1416,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1501,7 +1522,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1643,7 +1664,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1657,34 +1678,34 @@
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.54296875" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" customWidth="1"/>
-    <col min="4" max="6" width="12.81640625" style="105" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="6" width="12.85546875" style="105" customWidth="1"/>
     <col min="7" max="11" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="114" t="s">
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="126" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="111" t="s">
+      <c r="D4" s="123" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="113"/>
-      <c r="H4" s="116" t="s">
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="125"/>
+      <c r="H4" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="I4" s="112"/>
-      <c r="J4" s="112"/>
-      <c r="K4" s="113"/>
-    </row>
-    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="115"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="125"/>
+    </row>
+    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="127"/>
       <c r="D5" s="106" t="s">
         <v>129</v>
       </c>
@@ -1710,7 +1731,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C6" s="57" t="s">
         <v>84</v>
       </c>
@@ -1731,7 +1752,7 @@
       <c r="J6" s="75"/>
       <c r="K6" s="57"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C7" s="54" t="s">
         <v>85</v>
       </c>
@@ -1752,7 +1773,7 @@
       <c r="J7" s="76"/>
       <c r="K7" s="54"/>
     </row>
-    <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="55" t="s">
         <v>86</v>
       </c>
@@ -1773,7 +1794,7 @@
       <c r="J8" s="77"/>
       <c r="K8" s="55"/>
     </row>
-    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="72"/>
       <c r="D9" s="106"/>
       <c r="E9" s="107"/>
@@ -1784,8 +1805,8 @@
       <c r="J9" s="2"/>
       <c r="K9" s="72"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B10" s="110" t="s">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="122" t="s">
         <v>88</v>
       </c>
       <c r="C10" s="57" t="s">
@@ -1800,8 +1821,8 @@
       <c r="J10" s="75"/>
       <c r="K10" s="57"/>
     </row>
-    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="110"/>
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="122"/>
       <c r="C11" s="55" t="s">
         <v>84</v>
       </c>
@@ -1814,28 +1835,28 @@
       <c r="J11" s="77"/>
       <c r="K11" s="55"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="D14" s="110" t="s">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="122" t="s">
         <v>122</v>
       </c>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="110" t="s">
+      <c r="E14" s="122"/>
+      <c r="F14" s="122"/>
+      <c r="G14" s="122" t="s">
         <v>123</v>
       </c>
-      <c r="H14" s="110"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="110" t="s">
+      <c r="H14" s="122"/>
+      <c r="I14" s="122"/>
+      <c r="J14" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="110" t="s">
+      <c r="K14" s="122" t="s">
         <v>11</v>
       </c>
-      <c r="L14" s="110" t="s">
+      <c r="L14" s="122" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D15" s="44" t="s">
         <v>124</v>
       </c>
@@ -1854,9 +1875,9 @@
       <c r="I15" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="J15" s="110"/>
-      <c r="K15" s="110"/>
-      <c r="L15" s="110"/>
+      <c r="J15" s="122"/>
+      <c r="K15" s="122"/>
+      <c r="L15" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1882,22 +1903,22 @@
       <selection activeCell="E1" sqref="E1:M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.36328125" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="6" width="5.453125" style="1"/>
-    <col min="7" max="7" width="6.08984375" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.453125" style="1"/>
-    <col min="12" max="12" width="4.1796875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="5.26953125" customWidth="1"/>
-    <col min="14" max="14" width="55.26953125" customWidth="1"/>
+    <col min="5" max="6" width="5.42578125" style="1"/>
+    <col min="7" max="7" width="6.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" style="1"/>
+    <col min="12" max="12" width="4.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="5.28515625" customWidth="1"/>
+    <col min="14" max="14" width="55.28515625" customWidth="1"/>
     <col min="15" max="15" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
         <v>114</v>
       </c>
@@ -1910,23 +1931,23 @@
       <c r="D1" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="117" t="s">
+      <c r="E1" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="117"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="119" t="s">
+      <c r="F1" s="129"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="117"/>
-      <c r="J1" s="118"/>
-      <c r="K1" s="119" t="s">
+      <c r="I1" s="129"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="117"/>
-      <c r="M1" s="118"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L1" s="129"/>
+      <c r="M1" s="130"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
         <v>26</v>
       </c>
@@ -1968,7 +1989,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
         <v>27</v>
       </c>
@@ -2010,7 +2031,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
         <v>28</v>
       </c>
@@ -2052,7 +2073,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
         <v>29</v>
       </c>
@@ -2094,7 +2115,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="79" t="s">
         <v>30</v>
       </c>
@@ -2136,7 +2157,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
         <v>62</v>
       </c>
@@ -2177,7 +2198,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="80" t="s">
         <v>116</v>
       </c>
@@ -2224,7 +2245,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="80" t="s">
         <v>64</v>
       </c>
@@ -2271,7 +2292,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
         <v>65</v>
       </c>
@@ -2312,7 +2333,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
         <v>66</v>
       </c>
@@ -2353,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
         <v>67</v>
       </c>
@@ -2394,7 +2415,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
         <v>68</v>
       </c>
@@ -2438,7 +2459,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
         <v>69</v>
       </c>
@@ -2485,7 +2506,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
         <v>70</v>
       </c>
@@ -2529,7 +2550,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
         <v>71</v>
       </c>
@@ -2573,7 +2594,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="39" t="s">
         <v>72</v>
       </c>
@@ -2617,7 +2638,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
         <v>73</v>
       </c>
@@ -2661,7 +2682,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
         <v>74</v>
       </c>
@@ -2705,7 +2726,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="44" t="s">
         <v>75</v>
       </c>
@@ -2749,7 +2770,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="s">
         <v>76</v>
       </c>
@@ -2793,7 +2814,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="44"/>
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
@@ -2804,7 +2825,7 @@
       <c r="K22" s="6"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="44" t="s">
         <v>33</v>
       </c>
@@ -2826,7 +2847,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="44"/>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -2846,7 +2867,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D25" s="3"/>
       <c r="H25" s="2" t="s">
         <v>8</v>
@@ -2858,7 +2879,7 @@
       <c r="K25" s="6"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D26" s="3"/>
       <c r="H26" s="2" t="s">
         <v>15</v>
@@ -2870,7 +2891,7 @@
       <c r="K26" s="6"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D27" s="3"/>
       <c r="H27" s="2" t="s">
         <v>8</v>
@@ -2882,38 +2903,38 @@
       <c r="K27" s="6"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D28" s="3"/>
       <c r="H28" s="2"/>
       <c r="J28" s="3"/>
       <c r="K28" s="6"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D29" s="3"/>
       <c r="H29" s="2"/>
       <c r="J29" s="3"/>
       <c r="K29" s="6"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D30" s="3"/>
       <c r="H30" s="2"/>
       <c r="J30" s="3"/>
       <c r="K30" s="6"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D31" s="3"/>
       <c r="H31" s="2"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D32" s="3"/>
       <c r="H32" s="2"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D33" s="3"/>
       <c r="H33" s="2"/>
       <c r="J33" s="3"/>
@@ -2934,19 +2955,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68E12D-C9CD-4DEC-A7DD-D60B42882618}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" style="50" customWidth="1"/>
-    <col min="2" max="4" width="17.26953125" style="50" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" style="50" customWidth="1"/>
-    <col min="6" max="16384" width="29.81640625" style="50"/>
+    <col min="1" max="1" width="19.85546875" style="50" customWidth="1"/>
+    <col min="2" max="4" width="17.28515625" style="50" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="50" customWidth="1"/>
+    <col min="6" max="16384" width="29.85546875" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="59" t="s">
         <v>114</v>
       </c>
@@ -2963,7 +2984,7 @@
       <c r="F1" s="61"/>
       <c r="G1" s="62"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="63"/>
       <c r="B2" s="50" t="s">
         <v>42</v>
@@ -2979,7 +3000,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="63"/>
       <c r="B3" s="50" t="s">
         <v>43</v>
@@ -2995,7 +3016,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="63"/>
       <c r="B4" s="50" t="s">
         <v>44</v>
@@ -3011,7 +3032,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
       <c r="B5" s="50" t="s">
         <v>45</v>
@@ -3027,7 +3048,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="63"/>
       <c r="B6" s="50" t="s">
         <v>46</v>
@@ -3043,7 +3064,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="63"/>
       <c r="B7" s="50" t="s">
         <v>47</v>
@@ -3059,7 +3080,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
       <c r="B8" s="90" t="s">
         <v>48</v>
@@ -3080,7 +3101,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="63"/>
       <c r="B9" s="50" t="s">
         <v>49</v>
@@ -3096,7 +3117,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63"/>
       <c r="B10" s="50" t="s">
         <v>50</v>
@@ -3112,24 +3133,28 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="68" t="s">
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="133" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="134" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="61" t="s">
+      <c r="C11" s="134" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="62" t="s">
+      <c r="D11" s="135" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="62"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E11" s="134"/>
+      <c r="F11" s="134"/>
+      <c r="G11" s="135"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="65" t="s">
         <v>78</v>
       </c>
@@ -3156,23 +3181,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD31B0A-8ACD-468E-8C67-02F9624BD3CF}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" style="50" customWidth="1"/>
-    <col min="2" max="2" width="16.90625" style="50" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" style="50" customWidth="1"/>
-    <col min="4" max="4" width="23.1796875" style="50" customWidth="1"/>
-    <col min="5" max="13" width="6.453125" style="50" customWidth="1"/>
-    <col min="14" max="14" width="24.6328125" style="50" customWidth="1"/>
-    <col min="15" max="15" width="16.36328125" style="50" customWidth="1"/>
-    <col min="16" max="16384" width="29.81640625" style="50"/>
+    <col min="1" max="1" width="18.85546875" style="50" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="50" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="50" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="50" customWidth="1"/>
+    <col min="5" max="13" width="6.42578125" style="50" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" style="50" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" style="50" customWidth="1"/>
+    <col min="16" max="16384" width="29.85546875" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="59" t="s">
         <v>114</v>
       </c>
@@ -3207,7 +3232,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">
         <v>108</v>
       </c>
@@ -3220,41 +3245,41 @@
       <c r="D2" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="120" t="s">
+      <c r="E2" s="110" t="s">
         <v>139</v>
       </c>
-      <c r="F2" s="120" t="s">
+      <c r="F2" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="121">
+      <c r="G2" s="111">
         <v>8</v>
       </c>
-      <c r="H2" s="122" t="s">
+      <c r="H2" s="112" t="s">
         <v>142</v>
       </c>
-      <c r="I2" s="123" t="s">
+      <c r="I2" s="113" t="s">
         <v>143</v>
       </c>
-      <c r="J2" s="124">
+      <c r="J2" s="114">
         <v>3</v>
       </c>
-      <c r="K2" s="125" t="s">
+      <c r="K2" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="120" t="s">
+      <c r="L2" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="124">
+      <c r="M2" s="114">
         <v>0</v>
       </c>
-      <c r="N2" s="133">
+      <c r="N2">
         <v>231</v>
       </c>
-      <c r="O2" s="133">
+      <c r="O2">
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="63" t="s">
         <v>109</v>
       </c>
@@ -3267,41 +3292,41 @@
       <c r="D3" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="120" t="s">
+      <c r="E3" s="110" t="s">
         <v>140</v>
       </c>
-      <c r="F3" s="120" t="s">
+      <c r="F3" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="121">
+      <c r="G3" s="111">
         <v>12</v>
       </c>
-      <c r="H3" s="122" t="s">
+      <c r="H3" s="112" t="s">
         <v>142</v>
       </c>
-      <c r="I3" s="123" t="s">
+      <c r="I3" s="113" t="s">
         <v>143</v>
       </c>
-      <c r="J3" s="124">
+      <c r="J3" s="114">
         <v>10</v>
       </c>
-      <c r="K3" s="125" t="s">
+      <c r="K3" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="120" t="s">
+      <c r="L3" s="110" t="s">
         <v>144</v>
       </c>
-      <c r="M3" s="124">
+      <c r="M3" s="114">
         <v>23</v>
       </c>
-      <c r="N3" s="133">
+      <c r="N3">
         <v>112</v>
       </c>
-      <c r="O3" s="133">
+      <c r="O3">
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="63" t="s">
         <v>110</v>
       </c>
@@ -3314,41 +3339,41 @@
       <c r="D4" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="E4" s="120" t="s">
+      <c r="E4" s="110" t="s">
         <v>139</v>
       </c>
-      <c r="F4" s="120" t="s">
+      <c r="F4" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="121">
+      <c r="G4" s="111">
         <v>20</v>
       </c>
-      <c r="H4" s="122" t="s">
+      <c r="H4" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="123" t="s">
+      <c r="I4" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="124">
+      <c r="J4" s="114">
         <v>9</v>
       </c>
-      <c r="K4" s="125" t="s">
+      <c r="K4" s="115" t="s">
         <v>142</v>
       </c>
-      <c r="L4" s="120" t="s">
+      <c r="L4" s="110" t="s">
         <v>145</v>
       </c>
-      <c r="M4" s="124">
+      <c r="M4" s="114">
         <v>25</v>
       </c>
-      <c r="N4" s="133">
+      <c r="N4">
         <v>100</v>
       </c>
-      <c r="O4" s="133">
+      <c r="O4">
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
         <v>135</v>
       </c>
@@ -3361,41 +3386,41 @@
       <c r="D5" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="120" t="s">
+      <c r="E5" s="110" t="s">
         <v>139</v>
       </c>
-      <c r="F5" s="120" t="s">
+      <c r="F5" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="G5" s="121">
+      <c r="G5" s="111">
         <v>9</v>
       </c>
-      <c r="H5" s="122" t="s">
+      <c r="H5" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="123" t="s">
+      <c r="I5" s="113" t="s">
         <v>143</v>
       </c>
-      <c r="J5" s="124">
+      <c r="J5" s="114">
         <v>11</v>
       </c>
-      <c r="K5" s="125" t="s">
+      <c r="K5" s="115" t="s">
         <v>142</v>
       </c>
-      <c r="L5" s="120" t="s">
+      <c r="L5" s="110" t="s">
         <v>145</v>
       </c>
-      <c r="M5" s="124">
+      <c r="M5" s="114">
         <v>38</v>
       </c>
-      <c r="N5" s="133">
+      <c r="N5">
         <v>80</v>
       </c>
-      <c r="O5" s="133">
+      <c r="O5">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="63" t="s">
         <v>137</v>
       </c>
@@ -3408,61 +3433,61 @@
       <c r="D6" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="126" t="s">
+      <c r="E6" s="116" t="s">
         <v>139</v>
       </c>
-      <c r="F6" s="126" t="s">
+      <c r="F6" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="127">
+      <c r="G6" s="117">
         <v>18</v>
       </c>
-      <c r="H6" s="128" t="s">
+      <c r="H6" s="118" t="s">
         <v>142</v>
       </c>
-      <c r="I6" s="129" t="s">
+      <c r="I6" s="119" t="s">
         <v>143</v>
       </c>
-      <c r="J6" s="130">
+      <c r="J6" s="120">
         <v>17</v>
       </c>
-      <c r="K6" s="131" t="s">
+      <c r="K6" s="121" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="126" t="s">
+      <c r="L6" s="116" t="s">
         <v>145</v>
       </c>
-      <c r="M6" s="130">
+      <c r="M6" s="120">
         <v>19</v>
       </c>
-      <c r="N6" s="133">
+      <c r="N6">
         <v>35</v>
       </c>
-      <c r="O6" s="133">
+      <c r="O6">
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="63"/>
       <c r="D7" s="64"/>
       <c r="G7" s="64"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="63"/>
       <c r="D8" s="64"/>
       <c r="G8" s="64"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="63"/>
       <c r="D9" s="64"/>
       <c r="G9" s="64"/>
     </row>
-    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63"/>
       <c r="D10" s="64"/>
       <c r="G10" s="64"/>
     </row>
-    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="68"/>
       <c r="B11" s="61"/>
       <c r="C11" s="61"/>
@@ -3474,7 +3499,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="65"/>
       <c r="B12" s="66"/>
       <c r="C12" s="66"/>
@@ -3499,7 +3524,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3511,7 +3536,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Scatter plot for open vs close
</commit_message>
<xml_diff>
--- a/sessions_summary.xlsx
+++ b/sessions_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pri\Storage\Projects\ThalamoCorticalNetwork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Storage\MATLAB\ThalamocorticalLoop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF86137-160F-4FE0-9358-900430DDCBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C42A3A-14D8-4719-97C2-E0E4F1E4A65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{56367E76-6CBF-4746-8F91-48887379FCA8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{56367E76-6CBF-4746-8F91-48887379FCA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -20,28 +20,17 @@
     <sheet name="Lemmy-Kaining" sheetId="3" r:id="rId5"/>
     <sheet name="Slayer-Kaining" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="152">
   <si>
     <t>P3</t>
   </si>
@@ -491,6 +480,12 @@
   </si>
   <si>
     <t>Excluded: Post no eye-close</t>
+  </si>
+  <si>
+    <t>~300</t>
+  </si>
+  <si>
+    <t>~400</t>
   </si>
 </sst>
 </file>
@@ -1317,42 +1312,42 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1376,9 +1371,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1416,7 +1411,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1522,7 +1517,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1664,7 +1659,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1674,38 +1669,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E51CD7-F882-46FB-A302-DE4F0A9E1B83}">
   <dimension ref="B3:L15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="6" width="12.85546875" style="105" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" customWidth="1"/>
+    <col min="4" max="6" width="12.81640625" style="105" customWidth="1"/>
     <col min="7" max="11" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="126" t="s">
+    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="129" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="123" t="s">
+      <c r="D4" s="126" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="125"/>
-      <c r="H4" s="128" t="s">
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="125"/>
-    </row>
-    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="128"/>
+    </row>
+    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C5" s="130"/>
       <c r="D5" s="106" t="s">
         <v>129</v>
       </c>
@@ -1731,7 +1726,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C6" s="57" t="s">
         <v>84</v>
       </c>
@@ -1752,7 +1747,7 @@
       <c r="J6" s="75"/>
       <c r="K6" s="57"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C7" s="54" t="s">
         <v>85</v>
       </c>
@@ -1773,7 +1768,7 @@
       <c r="J7" s="76"/>
       <c r="K7" s="54"/>
     </row>
-    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C8" s="55" t="s">
         <v>86</v>
       </c>
@@ -1781,20 +1776,20 @@
         <v>0</v>
       </c>
       <c r="E8" s="100">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F8" s="101" t="s">
         <v>132</v>
       </c>
       <c r="G8" s="102">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H8" s="56"/>
       <c r="I8" s="71"/>
       <c r="J8" s="77"/>
       <c r="K8" s="55"/>
     </row>
-    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="72"/>
       <c r="D9" s="106"/>
       <c r="E9" s="107"/>
@@ -1805,8 +1800,8 @@
       <c r="J9" s="2"/>
       <c r="K9" s="72"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="122" t="s">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B10" s="125" t="s">
         <v>88</v>
       </c>
       <c r="C10" s="57" t="s">
@@ -1815,48 +1810,52 @@
       <c r="D10" s="92"/>
       <c r="E10" s="93"/>
       <c r="F10" s="94"/>
-      <c r="G10" s="57"/>
+      <c r="G10" s="57" t="s">
+        <v>150</v>
+      </c>
       <c r="H10" s="58"/>
       <c r="I10" s="74"/>
       <c r="J10" s="75"/>
       <c r="K10" s="57"/>
     </row>
-    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="122"/>
+    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="125"/>
       <c r="C11" s="55" t="s">
         <v>84</v>
       </c>
       <c r="D11" s="99"/>
       <c r="E11" s="100"/>
       <c r="F11" s="101"/>
-      <c r="G11" s="55"/>
+      <c r="G11" s="55" t="s">
+        <v>151</v>
+      </c>
       <c r="H11" s="56"/>
       <c r="I11" s="71"/>
       <c r="J11" s="77"/>
       <c r="K11" s="55"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D14" s="122" t="s">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="D14" s="125" t="s">
         <v>122</v>
       </c>
-      <c r="E14" s="122"/>
-      <c r="F14" s="122"/>
-      <c r="G14" s="122" t="s">
+      <c r="E14" s="125"/>
+      <c r="F14" s="125"/>
+      <c r="G14" s="125" t="s">
         <v>123</v>
       </c>
-      <c r="H14" s="122"/>
-      <c r="I14" s="122"/>
-      <c r="J14" s="122" t="s">
+      <c r="H14" s="125"/>
+      <c r="I14" s="125"/>
+      <c r="J14" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="122" t="s">
+      <c r="K14" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="L14" s="122" t="s">
+      <c r="L14" s="125" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="D15" s="44" t="s">
         <v>124</v>
       </c>
@@ -1875,9 +1874,9 @@
       <c r="I15" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="J15" s="122"/>
-      <c r="K15" s="122"/>
-      <c r="L15" s="122"/>
+      <c r="J15" s="125"/>
+      <c r="K15" s="125"/>
+      <c r="L15" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1899,26 +1898,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50FFE666-9548-4978-AD59-82159C4DB165}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="5.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="6" width="5.42578125" style="1"/>
-    <col min="7" max="7" width="6.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.42578125" style="1"/>
-    <col min="12" max="12" width="4.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="5.28515625" customWidth="1"/>
-    <col min="14" max="14" width="55.28515625" customWidth="1"/>
+    <col min="5" max="6" width="5.453125" style="1"/>
+    <col min="7" max="7" width="6.1796875" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.453125" style="1"/>
+    <col min="12" max="12" width="4.1796875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="5.26953125" customWidth="1"/>
+    <col min="14" max="14" width="55.26953125" customWidth="1"/>
     <col min="15" max="15" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="51" t="s">
         <v>114</v>
       </c>
@@ -1931,23 +1930,23 @@
       <c r="D1" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="129" t="s">
+      <c r="E1" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="129"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="131" t="s">
+      <c r="F1" s="132"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="129"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="131" t="s">
+      <c r="I1" s="132"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="134" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="129"/>
-      <c r="M1" s="130"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L1" s="132"/>
+      <c r="M1" s="133"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="44" t="s">
         <v>26</v>
       </c>
@@ -1989,7 +1988,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="44" t="s">
         <v>27</v>
       </c>
@@ -2031,7 +2030,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="44" t="s">
         <v>28</v>
       </c>
@@ -2073,7 +2072,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="44" t="s">
         <v>29</v>
       </c>
@@ -2115,7 +2114,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="79" t="s">
         <v>30</v>
       </c>
@@ -2157,7 +2156,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="44" t="s">
         <v>62</v>
       </c>
@@ -2198,7 +2197,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="80" t="s">
         <v>116</v>
       </c>
@@ -2245,7 +2244,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="80" t="s">
         <v>64</v>
       </c>
@@ -2292,7 +2291,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="44" t="s">
         <v>65</v>
       </c>
@@ -2333,7 +2332,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="44" t="s">
         <v>66</v>
       </c>
@@ -2374,7 +2373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="44" t="s">
         <v>67</v>
       </c>
@@ -2415,7 +2414,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="44" t="s">
         <v>68</v>
       </c>
@@ -2459,7 +2458,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="44" t="s">
         <v>69</v>
       </c>
@@ -2506,7 +2505,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="44" t="s">
         <v>70</v>
       </c>
@@ -2550,7 +2549,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="44" t="s">
         <v>71</v>
       </c>
@@ -2594,7 +2593,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="39" t="s">
         <v>72</v>
       </c>
@@ -2638,7 +2637,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="44" t="s">
         <v>73</v>
       </c>
@@ -2682,7 +2681,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="44" t="s">
         <v>74</v>
       </c>
@@ -2726,7 +2725,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="44" t="s">
         <v>75</v>
       </c>
@@ -2770,7 +2769,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="44" t="s">
         <v>76</v>
       </c>
@@ -2814,7 +2813,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="44"/>
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
@@ -2825,7 +2824,7 @@
       <c r="K22" s="6"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="44" t="s">
         <v>33</v>
       </c>
@@ -2847,7 +2846,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="44"/>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -2867,7 +2866,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D25" s="3"/>
       <c r="H25" s="2" t="s">
         <v>8</v>
@@ -2879,7 +2878,7 @@
       <c r="K25" s="6"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D26" s="3"/>
       <c r="H26" s="2" t="s">
         <v>15</v>
@@ -2891,7 +2890,7 @@
       <c r="K26" s="6"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D27" s="3"/>
       <c r="H27" s="2" t="s">
         <v>8</v>
@@ -2903,38 +2902,38 @@
       <c r="K27" s="6"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D28" s="3"/>
       <c r="H28" s="2"/>
       <c r="J28" s="3"/>
       <c r="K28" s="6"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D29" s="3"/>
       <c r="H29" s="2"/>
       <c r="J29" s="3"/>
       <c r="K29" s="6"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D30" s="3"/>
       <c r="H30" s="2"/>
       <c r="J30" s="3"/>
       <c r="K30" s="6"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D31" s="3"/>
       <c r="H31" s="2"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D32" s="3"/>
       <c r="H32" s="2"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D33" s="3"/>
       <c r="H33" s="2"/>
       <c r="J33" s="3"/>
@@ -2955,19 +2954,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68E12D-C9CD-4DEC-A7DD-D60B42882618}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="29.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="50" customWidth="1"/>
-    <col min="2" max="4" width="17.28515625" style="50" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="50" customWidth="1"/>
-    <col min="6" max="16384" width="29.85546875" style="50"/>
+    <col min="1" max="1" width="19.81640625" style="50" customWidth="1"/>
+    <col min="2" max="4" width="17.26953125" style="50" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" style="50" customWidth="1"/>
+    <col min="6" max="16384" width="29.81640625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="59" t="s">
         <v>114</v>
       </c>
@@ -2984,7 +2983,7 @@
       <c r="F1" s="61"/>
       <c r="G1" s="62"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="63"/>
       <c r="B2" s="50" t="s">
         <v>42</v>
@@ -3000,7 +2999,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="63"/>
       <c r="B3" s="50" t="s">
         <v>43</v>
@@ -3016,7 +3015,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="63"/>
       <c r="B4" s="50" t="s">
         <v>44</v>
@@ -3032,7 +3031,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="63"/>
       <c r="B5" s="50" t="s">
         <v>45</v>
@@ -3048,7 +3047,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="63"/>
       <c r="B6" s="50" t="s">
         <v>46</v>
@@ -3064,7 +3063,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="63"/>
       <c r="B7" s="50" t="s">
         <v>47</v>
@@ -3080,7 +3079,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="89"/>
       <c r="B8" s="90" t="s">
         <v>48</v>
@@ -3101,7 +3100,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="63"/>
       <c r="B9" s="50" t="s">
         <v>49</v>
@@ -3117,7 +3116,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="63"/>
       <c r="B10" s="50" t="s">
         <v>50</v>
@@ -3133,28 +3132,28 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="133" t="s">
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="122" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="134" t="s">
+      <c r="B11" s="123" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="134" t="s">
+      <c r="C11" s="123" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="135" t="s">
+      <c r="D11" s="124" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="134"/>
-      <c r="F11" s="134"/>
-      <c r="G11" s="135"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="124"/>
       <c r="H11" s="90"/>
       <c r="I11" s="90" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="65" t="s">
         <v>78</v>
       </c>
@@ -3182,22 +3181,22 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="G2" sqref="G2:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="29.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="50" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="50" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="50" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="50" customWidth="1"/>
-    <col min="5" max="13" width="6.42578125" style="50" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" style="50" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" style="50" customWidth="1"/>
-    <col min="16" max="16384" width="29.85546875" style="50"/>
+    <col min="1" max="1" width="18.81640625" style="50" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" style="50" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" style="50" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" style="50" customWidth="1"/>
+    <col min="5" max="13" width="6.453125" style="50" customWidth="1"/>
+    <col min="14" max="14" width="24.54296875" style="50" customWidth="1"/>
+    <col min="15" max="15" width="16.453125" style="50" customWidth="1"/>
+    <col min="16" max="16384" width="29.81640625" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="59" t="s">
         <v>114</v>
       </c>
@@ -3210,21 +3209,21 @@
       <c r="D1" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="132" t="s">
+      <c r="E1" s="135" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132" t="s">
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132" t="s">
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132"/>
+      <c r="L1" s="135"/>
+      <c r="M1" s="135"/>
       <c r="N1" s="50" t="s">
         <v>146</v>
       </c>
@@ -3232,7 +3231,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="63" t="s">
         <v>108</v>
       </c>
@@ -3279,7 +3278,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>109</v>
       </c>
@@ -3326,7 +3325,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="63" t="s">
         <v>110</v>
       </c>
@@ -3373,7 +3372,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="63" t="s">
         <v>135</v>
       </c>
@@ -3420,7 +3419,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="63" t="s">
         <v>137</v>
       </c>
@@ -3467,27 +3466,33 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="63"/>
-      <c r="D7" s="64"/>
+      <c r="D7" s="64" t="s">
+        <v>92</v>
+      </c>
       <c r="G7" s="64"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="63"/>
-      <c r="D8" s="64"/>
+      <c r="D8" s="64" t="s">
+        <v>93</v>
+      </c>
       <c r="G8" s="64"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="63"/>
-      <c r="D9" s="64"/>
+      <c r="D9" s="64" t="s">
+        <v>94</v>
+      </c>
       <c r="G9" s="64"/>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="63"/>
       <c r="D10" s="64"/>
       <c r="G10" s="64"/>
     </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="68"/>
       <c r="B11" s="61"/>
       <c r="C11" s="61"/>
@@ -3499,7 +3504,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="65"/>
       <c r="B12" s="66"/>
       <c r="C12" s="66"/>
@@ -3514,6 +3519,7 @@
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3524,7 +3530,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3536,7 +3542,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>